<commit_message>
updated data table & revision
</commit_message>
<xml_diff>
--- a/study 2 results.xlsx
+++ b/study 2 results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Desktop\my_proj\Online-Vid-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF35D8C-BB12-419B-AA1F-86E7D0C2A9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81805E94-59D2-4BE6-AE94-59E6E6F25CEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Interaction data" sheetId="1" r:id="rId1"/>
     <sheet name="1v2,2v2,3v3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,11 +71,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -84,6 +84,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -406,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection sqref="A1:I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -472,7 +479,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -501,7 +508,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -530,7 +537,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -559,7 +566,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -588,7 +595,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -617,7 +624,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -646,7 +653,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -675,7 +682,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -703,8 +710,12 @@
       <c r="I10" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <f>AVERAGE(E2:E25)</f>
+        <v>382.20833333333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -733,7 +744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -762,7 +773,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -791,7 +802,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -820,7 +831,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -849,7 +860,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -878,7 +889,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -907,7 +918,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -936,7 +947,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -965,7 +976,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>10</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -1023,7 +1034,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>11</v>
       </c>
@@ -1052,7 +1063,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -1081,7 +1092,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -1110,7 +1121,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>12</v>
       </c>
@@ -1139,7 +1150,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -1168,7 +1179,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1197,7 +1208,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1226,7 +1237,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1255,7 +1266,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -1284,7 +1295,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -1313,7 +1324,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -1342,7 +1353,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -1371,7 +1382,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>5</v>
       </c>
@@ -1400,7 +1411,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>5</v>
       </c>
@@ -1429,7 +1440,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>6</v>
       </c>
@@ -1458,7 +1469,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>6</v>
       </c>
@@ -1487,7 +1498,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>7</v>
       </c>
@@ -1516,7 +1527,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>7</v>
       </c>
@@ -1544,8 +1555,12 @@
       <c r="I39" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L39">
+        <f>AVERAGE(E26:E49)</f>
+        <v>474.70833333333331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>8</v>
       </c>
@@ -1574,7 +1589,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>8</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>9</v>
       </c>
@@ -1632,7 +1647,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>9</v>
       </c>
@@ -1661,7 +1676,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>10</v>
       </c>
@@ -1690,7 +1705,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>10</v>
       </c>
@@ -1719,7 +1734,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>11</v>
       </c>
@@ -1748,7 +1763,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>11</v>
       </c>
@@ -1777,7 +1792,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>12</v>
       </c>
@@ -1806,7 +1821,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>12</v>
       </c>
@@ -1836,7 +1851,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1848,8 +1865,9 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>